<commit_message>
fix: adjust results_concat file
</commit_message>
<xml_diff>
--- a/granularidade_grossa/results/rq2_table_best.xlsx
+++ b/granularidade_grossa/results/rq2_table_best.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,7 +494,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>gpt-4o-mini</t>
+          <t>mistral-nemo_12b</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -508,16 +508,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.78</v>
+        <v>0.71</v>
       </c>
       <c r="E2" t="n">
-        <v>0.49</v>
+        <v>0.48</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6</v>
+        <v>0.57</v>
       </c>
       <c r="G2" t="n">
-        <v>0.82</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3">
@@ -529,16 +529,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.74</v>
+        <v>0.61</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="F3" t="n">
-        <v>0.66</v>
+        <v>0.63</v>
       </c>
       <c r="G3" t="n">
-        <v>0.83</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="4">
@@ -554,16 +554,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.73</v>
+        <v>0.53</v>
       </c>
       <c r="E4" t="n">
-        <v>0.53</v>
+        <v>0.64</v>
       </c>
       <c r="F4" t="n">
-        <v>0.61</v>
+        <v>0.58</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="5">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.67</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7</v>
+        <v>0.68</v>
       </c>
       <c r="F5" t="n">
-        <v>0.68</v>
+        <v>0.61</v>
       </c>
       <c r="G5" t="n">
-        <v>0.82</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="6">
@@ -600,16 +600,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.74</v>
+        <v>0.55</v>
       </c>
       <c r="E6" t="n">
-        <v>0.53</v>
+        <v>0.6</v>
       </c>
       <c r="F6" t="n">
-        <v>0.62</v>
+        <v>0.57</v>
       </c>
       <c r="G6" t="n">
-        <v>0.82</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="7">
@@ -621,16 +621,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.71</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E7" t="n">
-        <v>0.63</v>
+        <v>0.6</v>
       </c>
       <c r="F7" t="n">
-        <v>0.67</v>
+        <v>0.58</v>
       </c>
       <c r="G7" t="n">
-        <v>0.82</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="8">
@@ -646,16 +646,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.75</v>
+        <v>0.71</v>
       </c>
       <c r="E8" t="n">
-        <v>0.51</v>
+        <v>0.44</v>
       </c>
       <c r="F8" t="n">
-        <v>0.61</v>
+        <v>0.55</v>
       </c>
       <c r="G8" t="n">
-        <v>0.82</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="9">
@@ -667,25 +667,218 @@
         </is>
       </c>
       <c r="D9" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>llama3.2_3b</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>zero_shot</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>Raw</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>Role-based</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>one_shot</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>Raw</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>Role-based</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n"/>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>few_shot</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>Raw</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="1" t="n"/>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>Role-based</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n"/>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>auto_cot</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>Raw</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n"/>
+      <c r="B17" s="1" t="n"/>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>Role-based</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="E17" t="n">
         <v>0.7</v>
       </c>
-      <c r="E9" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.82</v>
+      <c r="F17" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.73</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B12:B13"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A10:A17"/>
     <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>